<commit_message>
Pregnancy tests on lab results SDD
</commit_message>
<xml_diff>
--- a/metadata/SDD-NHANES-LAB-RESULTS.xlsx
+++ b/metadata/SDD-NHANES-LAB-RESULTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BF8D37-3A9A-3244-9D93-550D8BFA70F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F65F316-59B3-3247-A61E-8535DA60EAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10800" yWindow="-29420" windowWidth="26520" windowHeight="20100" activeTab="6" xr2:uid="{58E4DFD5-BA0B-AC44-8A63-99A3E8BCBB5B}"/>
+    <workbookView xWindow="1560" yWindow="500" windowWidth="26520" windowHeight="16760" activeTab="5" xr2:uid="{58E4DFD5-BA0B-AC44-8A63-99A3E8BCBB5B}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoSheet" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="85">
   <si>
     <t>Attribute</t>
   </si>
@@ -254,6 +254,48 @@
   </si>
   <si>
     <t>uo:0000165</t>
+  </si>
+  <si>
+    <t>??urine</t>
+  </si>
+  <si>
+    <t>uberon:0001088</t>
+  </si>
+  <si>
+    <t>??mec</t>
+  </si>
+  <si>
+    <t>nhanes:00027</t>
+  </si>
+  <si>
+    <t>URXPREG</t>
+  </si>
+  <si>
+    <t>nhanes:00116</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Not Done</t>
+  </si>
+  <si>
+    <t>nhanes:00117</t>
+  </si>
+  <si>
+    <t>nhanes:00118</t>
+  </si>
+  <si>
+    <t>nhanes:00119</t>
+  </si>
+  <si>
+    <t>nhanes:00120</t>
   </si>
 </sst>
 </file>
@@ -275,15 +317,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -291,12 +339,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,9 +914,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49E2EEE-9405-3D4B-BE45-6C4EFC175910}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -873,6 +943,62 @@
         <v>40</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -882,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74AF1B34-263D-2E4C-9E98-78435580EE88}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -958,57 +1084,59 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I4" t="s">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H5" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>56</v>
+        <v>71</v>
+      </c>
+      <c r="F6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" t="s">
+        <v>62</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="H7" t="s">
         <v>57</v>
@@ -1019,7 +1147,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
         <v>55</v>
@@ -1031,15 +1159,15 @@
         <v>56</v>
       </c>
       <c r="I8" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
         <v>57</v>
@@ -1050,7 +1178,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
         <v>55</v>
@@ -1059,10 +1187,58 @@
         <v>50</v>
       </c>
       <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
         <v>70</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I12" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included ucm, uio, vid, hepb
</commit_message>
<xml_diff>
--- a/metadata/SDD-NHANES-LAB-RESULTS.xlsx
+++ b/metadata/SDD-NHANES-LAB-RESULTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asthapatra/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F65F316-59B3-3247-A61E-8535DA60EAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC96EDEA-0425-F247-A677-5CF02525F7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="500" windowWidth="26520" windowHeight="16760" activeTab="5" xr2:uid="{58E4DFD5-BA0B-AC44-8A63-99A3E8BCBB5B}"/>
+    <workbookView xWindow="1100" yWindow="500" windowWidth="32440" windowHeight="20500" activeTab="6" xr2:uid="{58E4DFD5-BA0B-AC44-8A63-99A3E8BCBB5B}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoSheet" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="106">
   <si>
     <t>Attribute</t>
   </si>
@@ -296,6 +296,69 @@
   </si>
   <si>
     <t>nhanes:00120</t>
+  </si>
+  <si>
+    <t>??vic</t>
+  </si>
+  <si>
+    <t>LBXVIC</t>
+  </si>
+  <si>
+    <t>chebi:176783</t>
+  </si>
+  <si>
+    <t>URXUCM</t>
+  </si>
+  <si>
+    <t>sio:SIO_</t>
+  </si>
+  <si>
+    <t>??ucm</t>
+  </si>
+  <si>
+    <t>chebi: 33007</t>
+  </si>
+  <si>
+    <t>??ins</t>
+  </si>
+  <si>
+    <t>LBXIN</t>
+  </si>
+  <si>
+    <t>sio:SIO</t>
+  </si>
+  <si>
+    <t>chebi:145180</t>
+  </si>
+  <si>
+    <t>??isn</t>
+  </si>
+  <si>
+    <t>WTSA2YR</t>
+  </si>
+  <si>
+    <t>??uio</t>
+  </si>
+  <si>
+    <t>chebi:33115</t>
+  </si>
+  <si>
+    <t>??vid</t>
+  </si>
+  <si>
+    <t>LBXVIDMS</t>
+  </si>
+  <si>
+    <t>chebi:27300</t>
+  </si>
+  <si>
+    <t>??hepb</t>
+  </si>
+  <si>
+    <t>LBXHBC</t>
+  </si>
+  <si>
+    <t>LBXBHS</t>
   </si>
 </sst>
 </file>
@@ -916,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49E2EEE-9405-3D4B-BE45-6C4EFC175910}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1008,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74AF1B34-263D-2E4C-9E98-78435580EE88}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1241,6 +1304,164 @@
         <v>71</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" t="s">
+        <v>95</v>
+      </c>
+      <c r="I18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" t="s">
+        <v>102</v>
+      </c>
+      <c r="I22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished New Changing Data Lab Results
</commit_message>
<xml_diff>
--- a/metadata/SDD-NHANES-LAB-RESULTS.xlsx
+++ b/metadata/SDD-NHANES-LAB-RESULTS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asthapatra/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asthapatra/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC96EDEA-0425-F247-A677-5CF02525F7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F8AFB6-EDE9-D446-A7CE-302C8131EEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="500" windowWidth="32440" windowHeight="20500" activeTab="6" xr2:uid="{58E4DFD5-BA0B-AC44-8A63-99A3E8BCBB5B}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="110">
   <si>
     <t>Attribute</t>
   </si>
@@ -310,9 +310,6 @@
     <t>URXUCM</t>
   </si>
   <si>
-    <t>sio:SIO_</t>
-  </si>
-  <si>
     <t>??ucm</t>
   </si>
   <si>
@@ -322,12 +319,6 @@
     <t>??ins</t>
   </si>
   <si>
-    <t>LBXIN</t>
-  </si>
-  <si>
-    <t>sio:SIO</t>
-  </si>
-  <si>
     <t>chebi:145180</t>
   </si>
   <si>
@@ -352,13 +343,34 @@
     <t>chebi:27300</t>
   </si>
   <si>
-    <t>??hepb</t>
-  </si>
-  <si>
     <t>LBXHBC</t>
   </si>
   <si>
     <t>LBXBHS</t>
+  </si>
+  <si>
+    <t>uo:0000301</t>
+  </si>
+  <si>
+    <t>LBDHBG</t>
+  </si>
+  <si>
+    <t>LBDHD</t>
+  </si>
+  <si>
+    <t>ncit:C75678</t>
+  </si>
+  <si>
+    <t>ncit:C628795</t>
+  </si>
+  <si>
+    <t>ncit:C96664</t>
+  </si>
+  <si>
+    <t>uo:0000041</t>
+  </si>
+  <si>
+    <t>LBDNISI</t>
   </si>
 </sst>
 </file>
@@ -980,7 +992,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1071,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74AF1B34-263D-2E4C-9E98-78435580EE88}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1312,7 +1324,7 @@
         <v>87</v>
       </c>
       <c r="H14" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="I14" t="s">
         <v>50</v>
@@ -1337,10 +1349,13 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" t="s">
         <v>90</v>
       </c>
-      <c r="F16" t="s">
-        <v>91</v>
+      <c r="H16" t="s">
+        <v>62</v>
       </c>
       <c r="I16" t="s">
         <v>71</v>
@@ -1351,114 +1366,161 @@
         <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
         <v>71</v>
       </c>
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
       <c r="I17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" t="s">
         <v>92</v>
       </c>
-      <c r="F18" t="s">
-        <v>95</v>
+      <c r="H18" t="s">
+        <v>62</v>
       </c>
       <c r="I18" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" t="s">
         <v>93</v>
-      </c>
-      <c r="B19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F20" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="H20" t="s">
+        <v>62</v>
       </c>
       <c r="I20" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
         <v>71</v>
       </c>
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
       <c r="I21" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F22" t="s">
-        <v>102</v>
+        <v>99</v>
+      </c>
+      <c r="H22" t="s">
+        <v>57</v>
       </c>
       <c r="I22" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
         <v>50</v>
       </c>
+      <c r="D23" t="s">
+        <v>108</v>
+      </c>
       <c r="I23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>103</v>
-      </c>
-      <c r="I24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" t="s">
         <v>105</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added HEP B/D to Codebook
</commit_message>
<xml_diff>
--- a/metadata/SDD-NHANES-LAB-RESULTS.xlsx
+++ b/metadata/SDD-NHANES-LAB-RESULTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asthapatra/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F8AFB6-EDE9-D446-A7CE-302C8131EEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659E9F4F-0AF6-4141-8F00-06A2ECFE4337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="500" windowWidth="32440" windowHeight="20500" activeTab="6" xr2:uid="{58E4DFD5-BA0B-AC44-8A63-99A3E8BCBB5B}"/>
+    <workbookView xWindow="1100" yWindow="500" windowWidth="32440" windowHeight="20500" activeTab="5" xr2:uid="{58E4DFD5-BA0B-AC44-8A63-99A3E8BCBB5B}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoSheet" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="112">
   <si>
     <t>Attribute</t>
   </si>
@@ -358,19 +358,25 @@
     <t>LBDHD</t>
   </si>
   <si>
-    <t>ncit:C75678</t>
-  </si>
-  <si>
-    <t>ncit:C628795</t>
-  </si>
-  <si>
-    <t>ncit:C96664</t>
-  </si>
-  <si>
     <t>uo:0000041</t>
   </si>
   <si>
     <t>LBDNISI</t>
+  </si>
+  <si>
+    <t>nhanes:00154</t>
+  </si>
+  <si>
+    <t>obo:NCIT_C96664</t>
+  </si>
+  <si>
+    <t>obo: NCIT_C75678</t>
+  </si>
+  <si>
+    <t>obo: NCIT_C628795</t>
+  </si>
+  <si>
+    <t>Interdeterminate</t>
   </si>
 </sst>
 </file>
@@ -839,6 +845,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -862,6 +869,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -888,6 +896,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -923,6 +932,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -984,15 +994,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49E2EEE-9405-3D4B-BE45-6C4EFC175910}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1074,6 +1085,138 @@
         <v>84</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1085,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74AF1B34-263D-2E4C-9E98-78435580EE88}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1394,13 +1537,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
         <v>55</v>
       </c>
       <c r="C19" t="s">
         <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>107</v>
       </c>
       <c r="I19" t="s">
         <v>93</v>
@@ -1462,7 +1608,7 @@
         <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I23" t="s">
         <v>97</v>
@@ -1473,12 +1619,9 @@
         <v>100</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1487,12 +1630,9 @@
         <v>101</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
-      </c>
-      <c r="I26" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1501,12 +1641,9 @@
         <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
-      </c>
-      <c r="I27" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1515,16 +1652,14 @@
         <v>104</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C28" t="s">
         <v>50</v>
       </c>
-      <c r="I28" t="s">
-        <v>50</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>